<commit_message>
Kalberamatten Eintritte und Kiosk eingetragen
</commit_message>
<xml_diff>
--- a/Input/Verleiherabgaben.xlsx
+++ b/Input/Verleiherabgaben.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Kinoklub\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89BB4B7B-067D-479A-89FC-61FABFBA193F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D243FC7A-2410-40D3-AF34-7483C85D07A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="18696" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="18360" windowHeight="18576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Verleiherabgaben" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="169">
   <si>
     <t>Suisa</t>
   </si>
@@ -484,12 +484,6 @@
     <t>Kalbermatten</t>
   </si>
   <si>
-    <t>1005.027</t>
-  </si>
-  <si>
-    <t>TANGONACHT</t>
-  </si>
-  <si>
     <t>1020.295</t>
   </si>
   <si>
@@ -539,6 +533,18 @@
   </si>
   <si>
     <t>Rue Muzy 8</t>
+  </si>
+  <si>
+    <t>MovieBiz Films</t>
+  </si>
+  <si>
+    <t>Bachweg 18</t>
+  </si>
+  <si>
+    <t>1006.782</t>
+  </si>
+  <si>
+    <t>Cafe de los maestros</t>
   </si>
 </sst>
 </file>
@@ -818,8 +824,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{41B7D794-AABB-4EC4-84C2-1A317703EE4E}" name="Table1" displayName="Table1" ref="A1:E23" totalsRowShown="0" dataDxfId="5">
-  <autoFilter ref="A1:E23" xr:uid="{41B7D794-AABB-4EC4-84C2-1A317703EE4E}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{41B7D794-AABB-4EC4-84C2-1A317703EE4E}" name="Table1" displayName="Table1" ref="A1:E24" totalsRowShown="0" dataDxfId="5">
+  <autoFilter ref="A1:E24" xr:uid="{41B7D794-AABB-4EC4-84C2-1A317703EE4E}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A19">
     <sortCondition ref="A1:A51"/>
   </sortState>
@@ -1109,8 +1115,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E38" sqref="E38"/>
+    <sheetView tabSelected="1" topLeftCell="B19" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G42" sqref="G42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1130,7 +1136,7 @@
         <v>1</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
@@ -1683,7 +1689,7 @@
       </c>
       <c r="B27" s="12"/>
       <c r="C27" s="1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D27" s="6">
         <v>0</v>
@@ -1692,10 +1698,10 @@
         <v>30</v>
       </c>
       <c r="G27" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="H27" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.3">
@@ -1962,7 +1968,12 @@
       <c r="C40" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="E40" s="8"/>
+      <c r="D40" s="6">
+        <v>150</v>
+      </c>
+      <c r="E40" s="8">
+        <v>50</v>
+      </c>
       <c r="G40" t="s">
         <v>147</v>
       </c>
@@ -1976,11 +1987,14 @@
       </c>
       <c r="B41" s="12"/>
       <c r="C41" s="1" t="s">
-        <v>148</v>
+        <v>167</v>
       </c>
       <c r="E41" s="8"/>
+      <c r="F41">
+        <v>250</v>
+      </c>
       <c r="G41" t="s">
-        <v>149</v>
+        <v>168</v>
       </c>
       <c r="H41" t="s">
         <v>40</v>
@@ -1992,7 +2006,7 @@
       </c>
       <c r="B42" s="12"/>
       <c r="C42" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D42" s="6">
         <v>150</v>
@@ -2001,7 +2015,7 @@
         <v>30</v>
       </c>
       <c r="G42" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="H42" t="s">
         <v>42</v>
@@ -2013,7 +2027,7 @@
       </c>
       <c r="B43" s="12"/>
       <c r="C43" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D43" s="6">
         <v>150</v>
@@ -2022,10 +2036,10 @@
         <v>30</v>
       </c>
       <c r="G43" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="H43" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="44" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -2036,7 +2050,7 @@
       <c r="E44" s="8"/>
       <c r="F44" s="11"/>
       <c r="G44" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="45" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
@@ -2045,7 +2059,7 @@
       </c>
       <c r="B45" s="12"/>
       <c r="C45" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D45" s="6">
         <v>150</v>
@@ -2055,7 +2069,7 @@
       </c>
       <c r="F45" s="10"/>
       <c r="G45" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="H45" t="s">
         <v>41</v>
@@ -2086,10 +2100,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2012A76-D168-4BE0-9450-2E40BA8CE7CD}">
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView zoomScale="129" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2143,7 +2157,7 @@
         <v>24</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>77</v>
@@ -2460,13 +2474,13 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B22" s="4" t="s">
         <v>24</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D22" s="7" t="s">
         <v>64</v>
@@ -2477,19 +2491,36 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B23" s="4" t="s">
         <v>24</v>
       </c>
       <c r="C23" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="E23" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="D23" s="7" t="s">
-        <v>163</v>
-      </c>
-      <c r="E23" s="4" t="s">
-        <v>164</v>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -2505,7 +2536,7 @@
           <x14:formula1>
             <xm:f>dropdown!$A$2:$A$3</xm:f>
           </x14:formula1>
-          <xm:sqref>B2:B23</xm:sqref>
+          <xm:sqref>B2:B24</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
weihnachten 15.12.24 Eintritte, Kiosk, Show und Verleiherabgaben angepasst.
</commit_message>
<xml_diff>
--- a/Input/Verleiherabgaben.xlsx
+++ b/Input/Verleiherabgaben.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Kinoklub\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D243FC7A-2410-40D3-AF34-7483C85D07A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3508F3D-97B4-4D9A-B141-CEA90CAC148C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="18360" windowHeight="18576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2964" yWindow="1884" windowWidth="15684" windowHeight="11832" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Verleiherabgaben" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="170">
   <si>
     <t>Suisa</t>
   </si>
@@ -545,6 +545,9 @@
   </si>
   <si>
     <t>Cafe de los maestros</t>
+  </si>
+  <si>
+    <t>TAB0.108</t>
   </si>
 </sst>
 </file>
@@ -1115,8 +1118,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B19" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G42" sqref="G42"/>
+    <sheetView tabSelected="1" topLeftCell="A38" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E45" sqref="E45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2047,7 +2050,15 @@
         <v>45641</v>
       </c>
       <c r="B44" s="12"/>
-      <c r="E44" s="8"/>
+      <c r="C44" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="D44" s="6">
+        <v>150</v>
+      </c>
+      <c r="E44" s="8">
+        <v>47.7</v>
+      </c>
       <c r="F44" s="11"/>
       <c r="G44" t="s">
         <v>152</v>

</xml_diff>

<commit_message>
Eintritte und Kiosk für 10.1 & 17.1.25. Shows und Verleiherabgaben angepasst und Einnahmen Ausgaben angepasst.
</commit_message>
<xml_diff>
--- a/Input/Verleiherabgaben.xlsx
+++ b/Input/Verleiherabgaben.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\R Packages\Kinoklub\Input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Kinoklub\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC099508-1AC2-40A6-BC13-96317AD49EB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{445062CE-6899-4E16-81BD-1556440A4E50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17055" yWindow="4725" windowWidth="18645" windowHeight="12435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14220" yWindow="2676" windowWidth="15684" windowHeight="11832" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Verleiherabgaben" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="119">
   <si>
     <t>Suisa</t>
   </si>
@@ -61,9 +61,6 @@
     <t>nein</t>
   </si>
   <si>
-    <t>Ella und der Schwarze Jaguar</t>
-  </si>
-  <si>
     <t>Verleiher</t>
   </si>
   <si>
@@ -268,9 +265,6 @@
     <t>Baslerstrasse 30</t>
   </si>
   <si>
-    <t>1018.574</t>
-  </si>
-  <si>
     <t>Kein Verleiher</t>
   </si>
   <si>
@@ -280,12 +274,6 @@
     <t>0000</t>
   </si>
   <si>
-    <t>1016.779</t>
-  </si>
-  <si>
-    <t>FAMILIE: Harold und die Zauberkreide</t>
-  </si>
-  <si>
     <t>Sony Pictures Releasing Switzerland GmbH</t>
   </si>
   <si>
@@ -326,6 +314,87 @@
   </si>
   <si>
     <t>Ahrensfelde</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1020.828</t>
+  </si>
+  <si>
+    <t>1020.279</t>
+  </si>
+  <si>
+    <t>1020.643</t>
+  </si>
+  <si>
+    <t>1020.514</t>
+  </si>
+  <si>
+    <t>1020.563</t>
+  </si>
+  <si>
+    <t>1020.599</t>
+  </si>
+  <si>
+    <t>1020.566</t>
+  </si>
+  <si>
+    <t>1018.377</t>
+  </si>
+  <si>
+    <t>1019.343</t>
+  </si>
+  <si>
+    <t>1021.174</t>
+  </si>
+  <si>
+    <t>1020.652</t>
+  </si>
+  <si>
+    <t>1020.521</t>
+  </si>
+  <si>
+    <t>1019.051</t>
+  </si>
+  <si>
+    <t>Typisch Emil</t>
+  </si>
+  <si>
+    <t>The Outrun</t>
+  </si>
+  <si>
+    <t>Flow</t>
+  </si>
+  <si>
+    <t>Everybody Hates Johan</t>
+  </si>
+  <si>
+    <t>Wisdom of Happiness - A heart-to-heart with the Dalai Lama</t>
+  </si>
+  <si>
+    <t>The seed of the sacred fig</t>
+  </si>
+  <si>
+    <t>A Real Pain</t>
+  </si>
+  <si>
+    <t>The Missile</t>
+  </si>
+  <si>
+    <t>Lee - Die Fotografin</t>
+  </si>
+  <si>
+    <t>Die Drei ??? und der Karpatenhund</t>
+  </si>
+  <si>
+    <t>Hölde - die stillen Helden vom Säntis</t>
+  </si>
+  <si>
+    <t>Der Vierer</t>
+  </si>
+  <si>
+    <t>Die Witwe Clicquot</t>
+  </si>
+  <si>
+    <t>Gefangene des Schicksals (Zusammenarbeit mit Impuls Zusammenleben)</t>
   </si>
 </sst>
 </file>
@@ -336,7 +405,7 @@
     <numFmt numFmtId="164" formatCode="&quot;CHF&quot;\ #,##0.00"/>
     <numFmt numFmtId="165" formatCode="dd/mm/yyyy;@"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -362,6 +431,14 @@
       <color rgb="FF000000"/>
       <name val="Helvetica"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -371,7 +448,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -379,11 +456,40 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="dashed">
+        <color auto="1"/>
+      </left>
+      <right style="dashed">
+        <color auto="1"/>
+      </right>
+      <top style="dashed">
+        <color auto="1"/>
+      </top>
+      <bottom style="dashed">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dashed">
+        <color auto="1"/>
+      </left>
+      <right style="dashed">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="dashed">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -402,11 +508,14 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" xr:uid="{EB39806D-A340-4E6B-8E59-89A25516E3F2}"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="11">
+  <dxfs count="12">
     <dxf>
       <font>
         <b val="0"/>
@@ -530,6 +639,9 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="164" formatCode="&quot;CHF&quot;\ #,##0.00"/>
     </dxf>
     <dxf>
@@ -555,19 +667,19 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{0FB193BD-2953-40BE-9E24-FED98BF5CDC0}" name="Table3" displayName="Table3" ref="A1:H3" totalsRowShown="0">
-  <autoFilter ref="A1:H3" xr:uid="{0FB193BD-2953-40BE-9E24-FED98BF5CDC0}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{0FB193BD-2953-40BE-9E24-FED98BF5CDC0}" name="Table3" displayName="Table3" ref="A1:H15" totalsRowShown="0">
+  <autoFilter ref="A1:H15" xr:uid="{0FB193BD-2953-40BE-9E24-FED98BF5CDC0}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H3">
     <sortCondition ref="A1:A3"/>
   </sortState>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{DBD88967-C196-46D7-A0F4-D1ABEE204E92}" name="Datum" dataDxfId="10"/>
-    <tableColumn id="8" xr3:uid="{7055C330-D172-483B-B603-4A10F6395D71}" name="Link Datum" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{6B64E307-4A20-4FA5-9552-AEBC39618BBD}" name="Suisa" dataDxfId="8"/>
-    <tableColumn id="5" xr3:uid="{DCF2DA09-9338-4518-946C-A6B9B9132B96}" name="Minimal Abzug" dataDxfId="7"/>
+    <tableColumn id="1" xr3:uid="{DBD88967-C196-46D7-A0F4-D1ABEE204E92}" name="Datum" dataDxfId="11"/>
+    <tableColumn id="8" xr3:uid="{7055C330-D172-483B-B603-4A10F6395D71}" name="Link Datum" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{6B64E307-4A20-4FA5-9552-AEBC39618BBD}" name="Suisa" dataDxfId="9"/>
+    <tableColumn id="5" xr3:uid="{DCF2DA09-9338-4518-946C-A6B9B9132B96}" name="Minimal Abzug" dataDxfId="8"/>
     <tableColumn id="3" xr3:uid="{056159D4-E39B-4BCA-A63C-616B27132666}" name="Abzug [%]"/>
     <tableColumn id="4" xr3:uid="{3889FFD6-1D01-42CF-9D0C-73A343093947}" name="Abzug fix [CHF]"/>
-    <tableColumn id="6" xr3:uid="{7EA53B63-9001-4ABE-801A-79A1AD834F4D}" name="Titel"/>
+    <tableColumn id="6" xr3:uid="{7EA53B63-9001-4ABE-801A-79A1AD834F4D}" name="Titel" dataDxfId="7"/>
     <tableColumn id="7" xr3:uid="{0A2247CD-B246-49D9-B11E-A2EC995B4542}" name="Verleiher" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -864,36 +976,38 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="22.42578125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="10.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.42578125" style="5" customWidth="1"/>
-    <col min="5" max="5" width="16.28515625" customWidth="1"/>
-    <col min="6" max="6" width="20.5703125" customWidth="1"/>
-    <col min="7" max="7" width="43.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="43" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.77734375" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="61.77734375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="39" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="43" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E1" t="s">
         <v>2</v>
@@ -905,15 +1019,15 @@
         <v>3</v>
       </c>
       <c r="H1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
-        <v>45748</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>76</v>
+        <v>45667</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>92</v>
       </c>
       <c r="D2" s="5">
         <v>150</v>
@@ -921,32 +1035,294 @@
       <c r="E2" s="7">
         <v>30</v>
       </c>
+      <c r="F2"/>
       <c r="G2" t="s">
-        <v>7</v>
+        <v>105</v>
       </c>
       <c r="H2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
-        <v>45964</v>
+        <v>45674</v>
       </c>
       <c r="B3" s="8"/>
-      <c r="C3" s="1" t="s">
-        <v>80</v>
+      <c r="C3" s="10" t="s">
+        <v>93</v>
       </c>
       <c r="D3" s="5">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="E3" s="7">
         <v>30</v>
       </c>
+      <c r="F3"/>
       <c r="G3" t="s">
-        <v>81</v>
+        <v>106</v>
       </c>
       <c r="H3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="2">
+        <v>45676</v>
+      </c>
+      <c r="B4" s="8"/>
+      <c r="C4" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="D4" s="5">
+        <v>150</v>
+      </c>
+      <c r="E4" s="7">
+        <v>30</v>
+      </c>
+      <c r="F4"/>
+      <c r="G4" t="s">
+        <v>107</v>
+      </c>
+      <c r="H4" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="2">
+        <v>45682</v>
+      </c>
+      <c r="B5" s="8"/>
+      <c r="C5" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="D5" s="5">
+        <v>150</v>
+      </c>
+      <c r="E5" s="7">
+        <v>30</v>
+      </c>
+      <c r="F5"/>
+      <c r="G5" t="s">
+        <v>108</v>
+      </c>
+      <c r="H5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="2">
+        <v>45683</v>
+      </c>
+      <c r="B6" s="8"/>
+      <c r="C6" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="D6" s="5">
+        <v>150</v>
+      </c>
+      <c r="E6" s="7">
+        <v>30</v>
+      </c>
+      <c r="F6"/>
+      <c r="G6" t="s">
+        <v>109</v>
+      </c>
+      <c r="H6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" s="2">
+        <v>45683</v>
+      </c>
+      <c r="B7" s="8"/>
+      <c r="C7" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="D7" s="5"/>
+      <c r="E7" s="7"/>
+      <c r="F7"/>
+      <c r="G7" t="s">
+        <v>110</v>
+      </c>
+      <c r="H7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" s="2">
+        <v>45689</v>
+      </c>
+      <c r="B8" s="8"/>
+      <c r="C8" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="D8" s="5">
+        <v>150</v>
+      </c>
+      <c r="E8" s="7">
+        <v>30</v>
+      </c>
+      <c r="F8"/>
+      <c r="G8" t="s">
+        <v>111</v>
+      </c>
+      <c r="H8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" s="2">
+        <v>45689</v>
+      </c>
+      <c r="B9" s="8"/>
+      <c r="C9" s="10">
+        <v>1020.428</v>
+      </c>
+      <c r="D9" s="5">
+        <v>0</v>
+      </c>
+      <c r="E9" s="7">
+        <v>30</v>
+      </c>
+      <c r="F9"/>
+      <c r="G9" t="s">
+        <v>112</v>
+      </c>
+      <c r="H9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" s="2">
+        <v>45690</v>
+      </c>
+      <c r="B10" s="8"/>
+      <c r="C10" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="D10" s="5">
+        <v>150</v>
+      </c>
+      <c r="E10" s="7">
+        <v>30</v>
+      </c>
+      <c r="F10"/>
+      <c r="G10" t="s">
+        <v>113</v>
+      </c>
+      <c r="H10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" s="2">
+        <v>45690</v>
+      </c>
+      <c r="B11" s="8"/>
+      <c r="C11" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="D11" s="5">
+        <v>0</v>
+      </c>
+      <c r="E11" s="7">
+        <v>50</v>
+      </c>
+      <c r="F11"/>
+      <c r="G11" t="s">
+        <v>114</v>
+      </c>
+      <c r="H11" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" s="2">
+        <v>45690</v>
+      </c>
+      <c r="B12" s="8"/>
+      <c r="C12" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="D12" s="5">
+        <v>150</v>
+      </c>
+      <c r="E12" s="7">
+        <v>30</v>
+      </c>
+      <c r="F12"/>
+      <c r="G12" t="s">
+        <v>115</v>
+      </c>
+      <c r="H12" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" s="2">
+        <v>45695</v>
+      </c>
+      <c r="B13" s="8"/>
+      <c r="C13" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D13" s="5">
+        <v>150</v>
+      </c>
+      <c r="E13" s="7">
+        <v>30</v>
+      </c>
+      <c r="F13"/>
+      <c r="G13" t="s">
+        <v>116</v>
+      </c>
+      <c r="H13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" s="2">
+        <v>45701</v>
+      </c>
+      <c r="B14" s="8"/>
+      <c r="C14" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D14" s="5">
+        <v>0</v>
+      </c>
+      <c r="E14" s="7">
+        <v>30</v>
+      </c>
+      <c r="F14"/>
+      <c r="G14" t="s">
+        <v>117</v>
+      </c>
+      <c r="H14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" s="2">
+        <v>45738</v>
+      </c>
+      <c r="B15" s="8"/>
+      <c r="C15" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="D15" s="5">
+        <v>150</v>
+      </c>
+      <c r="E15" s="7">
+        <v>30</v>
+      </c>
+      <c r="F15"/>
+      <c r="G15" t="s">
+        <v>118</v>
+      </c>
+      <c r="H15" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -959,12 +1335,18 @@
   </tableParts>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{5BD6C4FD-BF72-41F7-85FD-AAAD92F80620}">
           <x14:formula1>
             <xm:f>'Kinoförderer gratis'!$A$2:$A$23</xm:f>
           </x14:formula1>
-          <xm:sqref>H2:H253</xm:sqref>
+          <xm:sqref>I16:I265</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{80937494-2B0B-4CA6-82E1-990B543FC73E}">
+          <x14:formula1>
+            <xm:f>'Kinoförderer gratis'!$A:$A</xm:f>
+          </x14:formula1>
+          <xm:sqref>H2:H15</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -977,453 +1359,453 @@
   <dimension ref="A1:E36"/>
   <sheetViews>
     <sheetView zoomScale="129" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="43.28515625" customWidth="1"/>
+    <col min="1" max="1" width="43.33203125" customWidth="1"/>
     <col min="2" max="2" width="20" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.88671875" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="B6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D7" s="6">
         <v>8057</v>
       </c>
       <c r="E7" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="D8" s="6" t="s">
+      <c r="D9" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A10" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="E8" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+      <c r="B10" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A13" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A17" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="D16" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C17" s="3" t="s">
+      <c r="B19" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="D17" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C18" s="3" t="s">
+      <c r="D19" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="D20" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="D18" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="D19" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C20" s="3" t="s">
+      <c r="E20" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="D20" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
+      <c r="B21" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="D21" s="6" t="s">
         <v>77</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="D21" s="6" t="s">
-        <v>79</v>
       </c>
       <c r="E21" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D23" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="B22" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="D22" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
+      <c r="E23" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="B23" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="D23" s="6" t="s">
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="E23" s="3" t="s">
+      <c r="B24" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C24" s="3" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
+      <c r="D24" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="D25" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="B24" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C24" s="3" t="s">
+      <c r="E25" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="D24" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="E24" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="D25" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="E25" s="3" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A33" s="9"/>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A34" s="9"/>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A35" s="9"/>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A36" s="9"/>
     </row>
   </sheetData>
@@ -1455,22 +1837,22 @@
       <selection activeCell="E47" sqref="E47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" customWidth="1"/>
+    <col min="1" max="1" width="11.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>

</xml_diff>

<commit_message>
Seed of sacred fig- Eintritte und Kiosk
</commit_message>
<xml_diff>
--- a/Input/Verleiherabgaben.xlsx
+++ b/Input/Verleiherabgaben.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\R Packages\Kinoklub\Input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Kinoklub\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7805E3E6-8A37-4782-B827-4E29F38049D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{437782EB-6C52-44C1-93EC-24B14FA5713C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15264" yWindow="0" windowWidth="15552" windowHeight="18576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Verleiherabgaben" sheetId="1" r:id="rId1"/>
@@ -513,12 +513,9 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" xr:uid="{EB39806D-A340-4E6B-8E59-89A25516E3F2}"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="12">
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -648,6 +645,9 @@
       <numFmt numFmtId="164" formatCode="&quot;CHF&quot;\ #,##0.00"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="165" formatCode="dd/mm/yyyy;@"/>
     </dxf>
     <dxf>
@@ -675,29 +675,29 @@
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{DBD88967-C196-46D7-A0F4-D1ABEE204E92}" name="Datum" dataDxfId="11"/>
     <tableColumn id="8" xr3:uid="{7055C330-D172-483B-B603-4A10F6395D71}" name="Link Datum" dataDxfId="10"/>
-    <tableColumn id="2" xr3:uid="{6B64E307-4A20-4FA5-9552-AEBC39618BBD}" name="Suisa" dataDxfId="0"/>
-    <tableColumn id="5" xr3:uid="{DCF2DA09-9338-4518-946C-A6B9B9132B96}" name="Minimal Abzug" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{6B64E307-4A20-4FA5-9552-AEBC39618BBD}" name="Suisa" dataDxfId="9"/>
+    <tableColumn id="5" xr3:uid="{DCF2DA09-9338-4518-946C-A6B9B9132B96}" name="Minimal Abzug" dataDxfId="8"/>
     <tableColumn id="3" xr3:uid="{056159D4-E39B-4BCA-A63C-616B27132666}" name="Abzug [%]"/>
     <tableColumn id="4" xr3:uid="{3889FFD6-1D01-42CF-9D0C-73A343093947}" name="Abzug fix [CHF]"/>
-    <tableColumn id="6" xr3:uid="{7EA53B63-9001-4ABE-801A-79A1AD834F4D}" name="Titel" dataDxfId="8"/>
-    <tableColumn id="7" xr3:uid="{0A2247CD-B246-49D9-B11E-A2EC995B4542}" name="Verleiher" dataDxfId="7"/>
+    <tableColumn id="6" xr3:uid="{7EA53B63-9001-4ABE-801A-79A1AD834F4D}" name="Titel" dataDxfId="7"/>
+    <tableColumn id="7" xr3:uid="{0A2247CD-B246-49D9-B11E-A2EC995B4542}" name="Verleiher" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{41B7D794-AABB-4EC4-84C2-1A317703EE4E}" name="Table1" displayName="Table1" ref="A1:E25" totalsRowShown="0" dataDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{41B7D794-AABB-4EC4-84C2-1A317703EE4E}" name="Table1" displayName="Table1" ref="A1:E25" totalsRowShown="0" dataDxfId="5">
   <autoFilter ref="A1:E25" xr:uid="{41B7D794-AABB-4EC4-84C2-1A317703EE4E}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A19">
     <sortCondition ref="A1:A51"/>
   </sortState>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{87B4203C-1728-449D-B1D9-EA610781FF80}" name="Verleiher" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{C3C9F269-200E-44AA-A999-C80DE0337772}" name="Kinoförderer gratis?" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{A3438286-188F-4B22-96EA-9046C8BD8738}" name="Adresse" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{4E36D4B9-CEC6-4204-8ACA-9F0B34AACC27}" name="PLZ" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{9871F211-6A68-4A87-B2B5-D2BD49D8C28F}" name="Ort" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{87B4203C-1728-449D-B1D9-EA610781FF80}" name="Verleiher" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{C3C9F269-200E-44AA-A999-C80DE0337772}" name="Kinoförderer gratis?" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{A3438286-188F-4B22-96EA-9046C8BD8738}" name="Adresse" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{4E36D4B9-CEC6-4204-8ACA-9F0B34AACC27}" name="PLZ" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{9871F211-6A68-4A87-B2B5-D2BD49D8C28F}" name="Ort" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -979,24 +979,24 @@
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.42578125" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.44140625" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="61.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="61.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="39" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="43" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -1022,7 +1022,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>45667</v>
       </c>
@@ -1043,7 +1043,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>45674</v>
       </c>
@@ -1065,7 +1065,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>45676</v>
       </c>
@@ -1087,7 +1087,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>45682</v>
       </c>
@@ -1109,7 +1109,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>45683</v>
       </c>
@@ -1131,7 +1131,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>45683</v>
       </c>
@@ -1139,8 +1139,12 @@
       <c r="C7" s="10" t="s">
         <v>97</v>
       </c>
-      <c r="D7" s="5"/>
-      <c r="E7" s="7"/>
+      <c r="D7" s="5">
+        <v>150</v>
+      </c>
+      <c r="E7" s="7">
+        <v>30</v>
+      </c>
       <c r="F7"/>
       <c r="G7" t="s">
         <v>110</v>
@@ -1149,7 +1153,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>45689</v>
       </c>
@@ -1171,7 +1175,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>45689</v>
       </c>
@@ -1193,7 +1197,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>45690</v>
       </c>
@@ -1215,7 +1219,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>45690</v>
       </c>
@@ -1237,7 +1241,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>45690</v>
       </c>
@@ -1259,7 +1263,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>45695</v>
       </c>
@@ -1281,7 +1285,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>45701</v>
       </c>
@@ -1303,7 +1307,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>45738</v>
       </c>
@@ -1362,16 +1366,16 @@
       <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="43.28515625" customWidth="1"/>
+    <col min="1" max="1" width="43.33203125" customWidth="1"/>
     <col min="2" max="2" width="20" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.88671875" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -1388,7 +1392,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>25</v>
       </c>
@@ -1405,7 +1409,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>21</v>
       </c>
@@ -1422,7 +1426,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>20</v>
       </c>
@@ -1439,7 +1443,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>53</v>
       </c>
@@ -1456,7 +1460,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>8</v>
       </c>
@@ -1473,7 +1477,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>11</v>
       </c>
@@ -1490,7 +1494,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>10</v>
       </c>
@@ -1507,7 +1511,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>12</v>
       </c>
@@ -1524,7 +1528,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>52</v>
       </c>
@@ -1541,7 +1545,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>15</v>
       </c>
@@ -1558,7 +1562,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>22</v>
       </c>
@@ -1575,7 +1579,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>19</v>
       </c>
@@ -1592,7 +1596,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>18</v>
       </c>
@@ -1609,7 +1613,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>16</v>
       </c>
@@ -1626,7 +1630,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>14</v>
       </c>
@@ -1643,7 +1647,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
         <v>17</v>
       </c>
@@ -1660,7 +1664,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>9</v>
       </c>
@@ -1677,7 +1681,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
         <v>13</v>
       </c>
@@ -1694,7 +1698,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>73</v>
       </c>
@@ -1711,7 +1715,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>75</v>
       </c>
@@ -1728,7 +1732,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>78</v>
       </c>
@@ -1745,7 +1749,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
         <v>79</v>
       </c>
@@ -1762,7 +1766,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
         <v>86</v>
       </c>
@@ -1779,7 +1783,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
         <v>88</v>
       </c>
@@ -1796,16 +1800,16 @@
         <v>91</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A33" s="9"/>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A34" s="9"/>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A35" s="9"/>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A36" s="9"/>
     </row>
   </sheetData>
@@ -1837,22 +1841,22 @@
       <selection activeCell="E47" sqref="E47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" customWidth="1"/>
+    <col min="1" max="1" width="11.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>

</xml_diff>